<commit_message>
move axis labels to bottom for conf_progression.xlsx
</commit_message>
<xml_diff>
--- a/results/conf_progression.xlsx
+++ b/results/conf_progression.xlsx
@@ -358,11 +358,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1759322752"/>
-        <c:axId val="-1759323296"/>
+        <c:axId val="-326970688"/>
+        <c:axId val="-326972320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1759322752"/>
+        <c:axId val="-326970688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,7 +425,7 @@
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="high"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -453,7 +453,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1759323296"/>
+        <c:crossAx val="-326972320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -461,7 +461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1759323296"/>
+        <c:axId val="-326972320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -561,7 +561,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1759322752"/>
+        <c:crossAx val="-326970688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -636,7 +636,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0" l="0" r="0" t="0" header="0" footer="0"/>
-    <c:pageSetup paperSize="32767" orientation="portrait"/>
+    <c:pageSetup paperSize="32767" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1412,7 +1412,7 @@
       <sheetName val="2016-11-07-4"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
           <cell r="D89">
@@ -1425,30 +1425,30 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>

<commit_message>
rm axis line in conf_progression.xlsx
</commit_message>
<xml_diff>
--- a/results/conf_progression.xlsx
+++ b/results/conf_progression.xlsx
@@ -358,11 +358,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-326970688"/>
-        <c:axId val="-326972320"/>
+        <c:axId val="-61743824"/>
+        <c:axId val="-61754704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-326970688"/>
+        <c:axId val="-61743824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -429,9 +429,7 @@
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:srgbClr val="868686"/>
-            </a:solidFill>
+            <a:noFill/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -453,7 +451,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-326972320"/>
+        <c:crossAx val="-61754704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -461,7 +459,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-326972320"/>
+        <c:axId val="-61754704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -561,7 +559,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-326970688"/>
+        <c:crossAx val="-61743824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -636,7 +634,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0" l="0" r="0" t="0" header="0" footer="0"/>
-    <c:pageSetup paperSize="32767" orientation="landscape"/>
+    <c:pageSetup paperSize="32767" orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2312,7 +2310,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>